<commit_message>
exhibitor estimated page modi
</commit_message>
<xml_diff>
--- a/final/data/VendorPriceSheet.xlsx
+++ b/final/data/VendorPriceSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangjiaqian/Desktop/git/1/final/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38387CD1-8336-C944-8181-ACB658703A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0335D324-AC39-084E-80A6-40C7974648B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14320" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="292">
   <si>
     <t>Category</t>
   </si>
@@ -4955,7 +4955,7 @@
   <dimension ref="A1:IV126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1"/>
@@ -5008,7 +5008,9 @@
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="14" customHeight="1">
-      <c r="A3" s="6"/>
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="5">
         <v>1.2</v>
       </c>
@@ -5023,7 +5025,9 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="14" customHeight="1">
-      <c r="A4" s="6"/>
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="5">
         <v>1.3</v>
       </c>
@@ -5038,7 +5042,9 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="14" customHeight="1">
-      <c r="A5" s="6"/>
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B5" s="5">
         <v>1.4</v>
       </c>
@@ -5053,7 +5059,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="14" customHeight="1">
-      <c r="A6" s="6"/>
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" s="5">
         <v>1.5</v>
       </c>
@@ -5068,7 +5076,9 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="14" customHeight="1">
-      <c r="A7" s="6"/>
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B7" s="5">
         <v>1.6</v>
       </c>
@@ -5083,7 +5093,9 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="14" customHeight="1">
-      <c r="A8" s="6"/>
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" s="5">
         <v>1.7</v>
       </c>
@@ -5115,7 +5127,9 @@
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="14" customHeight="1">
-      <c r="A10" s="6"/>
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4" t="s">
         <v>148</v>
@@ -5128,7 +5142,9 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="14" customHeight="1">
-      <c r="A11" s="6"/>
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B11" s="5">
         <v>2.2000000000000002</v>
       </c>
@@ -5143,7 +5159,9 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="14" customHeight="1">
-      <c r="A12" s="6"/>
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B12" s="5">
         <v>2.2999999999999998</v>
       </c>
@@ -5158,7 +5176,9 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="14" customHeight="1">
-      <c r="A13" s="6"/>
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B13" s="6"/>
       <c r="C13" s="4" t="s">
         <v>21</v>
@@ -5171,7 +5191,9 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="14" customHeight="1">
-      <c r="A14" s="6"/>
+      <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B14" s="5">
         <v>2.4</v>
       </c>
@@ -5186,7 +5208,9 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="14" customHeight="1">
-      <c r="A15" s="6"/>
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B15" s="5">
         <v>2.5</v>
       </c>
@@ -5201,7 +5225,9 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="14" customHeight="1">
-      <c r="A16" s="6"/>
+      <c r="A16" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B16" s="5">
         <v>2.6</v>
       </c>
@@ -5216,7 +5242,9 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="14" customHeight="1">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="B17" s="6"/>
       <c r="C17" s="4" t="s">
         <v>154</v>
@@ -5246,7 +5274,9 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="14" customHeight="1">
-      <c r="A19" s="6"/>
+      <c r="A19" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B19" s="6"/>
       <c r="C19" s="4" t="s">
         <v>30</v>
@@ -5259,7 +5289,9 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="14" customHeight="1">
-      <c r="A20" s="6"/>
+      <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B20" s="5">
         <v>3.2</v>
       </c>
@@ -5274,7 +5306,9 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="14" customHeight="1">
-      <c r="A21" s="6"/>
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
         <v>30</v>
@@ -5287,7 +5321,9 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="14" customHeight="1">
-      <c r="A22" s="6"/>
+      <c r="A22" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" s="5">
         <v>3.3</v>
       </c>
@@ -5302,7 +5338,9 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="14" customHeight="1">
-      <c r="A23" s="6"/>
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="6"/>
       <c r="C23" s="4" t="s">
         <v>30</v>
@@ -5315,7 +5353,9 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="14" customHeight="1">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" s="5">
         <v>3.4</v>
       </c>
@@ -5330,7 +5370,9 @@
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="14" customHeight="1">
-      <c r="A25" s="6"/>
+      <c r="A25" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" s="6"/>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -5343,7 +5385,9 @@
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="14" customHeight="1">
-      <c r="A26" s="6"/>
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="5">
         <v>3.5</v>
       </c>
@@ -5358,7 +5402,9 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="14" customHeight="1">
-      <c r="A27" s="6"/>
+      <c r="A27" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B27" s="6"/>
       <c r="C27" s="4" t="s">
         <v>30</v>
@@ -5371,7 +5417,9 @@
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="14" customHeight="1">
-      <c r="A28" s="6"/>
+      <c r="A28" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="5">
         <v>3.6</v>
       </c>
@@ -5386,7 +5434,9 @@
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="14" customHeight="1">
-      <c r="A29" s="6"/>
+      <c r="A29" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B29" s="6"/>
       <c r="C29" s="4" t="s">
         <v>30</v>
@@ -5399,7 +5449,9 @@
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="14" customHeight="1">
-      <c r="A30" s="6"/>
+      <c r="A30" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B30" s="5">
         <v>3.7</v>
       </c>
@@ -5414,7 +5466,9 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="14" customHeight="1">
-      <c r="A31" s="6"/>
+      <c r="A31" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B31" s="6"/>
       <c r="C31" s="4" t="s">
         <v>162</v>
@@ -5427,7 +5481,9 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="14" customHeight="1">
-      <c r="A32" s="6"/>
+      <c r="A32" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B32" s="5">
         <v>3.8</v>
       </c>
@@ -5442,7 +5498,9 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="14" customHeight="1">
-      <c r="A33" s="6"/>
+      <c r="A33" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B33" s="6"/>
       <c r="C33" s="4" t="s">
         <v>162</v>
@@ -5455,7 +5513,9 @@
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="14" customHeight="1">
-      <c r="A34" s="6"/>
+      <c r="A34" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B34" s="5">
         <v>3.9</v>
       </c>
@@ -5470,7 +5530,9 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="14" customHeight="1">
-      <c r="A35" s="6"/>
+      <c r="A35" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="B35" s="6"/>
       <c r="C35" s="4" t="s">
         <v>165</v>
@@ -5500,7 +5562,9 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="14" customHeight="1">
-      <c r="A37" s="6"/>
+      <c r="A37" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B37" s="6"/>
       <c r="C37" s="4" t="s">
         <v>167</v>
@@ -5513,7 +5577,9 @@
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="14" customHeight="1">
-      <c r="A38" s="6"/>
+      <c r="A38" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B38" s="6"/>
       <c r="C38" s="4" t="s">
         <v>168</v>
@@ -5526,7 +5592,9 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="14" customHeight="1">
-      <c r="A39" s="6"/>
+      <c r="A39" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B39" s="6"/>
       <c r="C39" s="4" t="s">
         <v>169</v>
@@ -5539,7 +5607,9 @@
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="14" customHeight="1">
-      <c r="A40" s="6"/>
+      <c r="A40" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B40" s="6"/>
       <c r="C40" s="4" t="s">
         <v>170</v>
@@ -5552,7 +5622,9 @@
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="14" customHeight="1">
-      <c r="A41" s="6"/>
+      <c r="A41" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B41" s="5">
         <v>4.2</v>
       </c>
@@ -5567,7 +5639,9 @@
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" ht="14" customHeight="1">
-      <c r="A42" s="6"/>
+      <c r="A42" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B42" s="6"/>
       <c r="C42" s="4" t="s">
         <v>172</v>
@@ -5580,7 +5654,9 @@
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" ht="14" customHeight="1">
-      <c r="A43" s="6"/>
+      <c r="A43" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B43" s="5">
         <v>4.3</v>
       </c>
@@ -5595,7 +5671,9 @@
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="14" customHeight="1">
-      <c r="A44" s="6"/>
+      <c r="A44" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B44" s="5">
         <v>4.4000000000000004</v>
       </c>
@@ -5610,7 +5688,9 @@
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="14" customHeight="1">
-      <c r="A45" s="6"/>
+      <c r="A45" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="B45" s="5">
         <v>4.5</v>
       </c>
@@ -5642,7 +5722,9 @@
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="14" customHeight="1">
-      <c r="A47" s="6"/>
+      <c r="A47" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B47" s="5">
         <v>5.2</v>
       </c>
@@ -5657,7 +5739,9 @@
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="14" customHeight="1">
-      <c r="A48" s="6"/>
+      <c r="A48" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B48" s="5">
         <v>5.3</v>
       </c>
@@ -5672,7 +5756,9 @@
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="14" customHeight="1">
-      <c r="A49" s="6"/>
+      <c r="A49" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B49" s="5">
         <v>5.4</v>
       </c>
@@ -5687,7 +5773,9 @@
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="14" customHeight="1">
-      <c r="A50" s="6"/>
+      <c r="A50" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B50" s="5">
         <v>5.5</v>
       </c>
@@ -5702,7 +5790,9 @@
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="14" customHeight="1">
-      <c r="A51" s="6"/>
+      <c r="A51" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B51" s="5">
         <v>5.6</v>
       </c>
@@ -5717,7 +5807,9 @@
       <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" ht="14" customHeight="1">
-      <c r="A52" s="6"/>
+      <c r="A52" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B52" s="5">
         <v>5.7</v>
       </c>
@@ -5732,7 +5824,9 @@
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" ht="14" customHeight="1">
-      <c r="A53" s="6"/>
+      <c r="A53" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B53" s="6"/>
       <c r="C53" s="4" t="s">
         <v>21</v>
@@ -5762,7 +5856,9 @@
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" ht="14" customHeight="1">
-      <c r="A55" s="6"/>
+      <c r="A55" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B55" s="5">
         <v>6.2</v>
       </c>
@@ -5777,7 +5873,9 @@
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="14" customHeight="1">
-      <c r="A56" s="6"/>
+      <c r="A56" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B56" s="5">
         <v>6.3</v>
       </c>
@@ -5792,7 +5890,9 @@
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" ht="14" customHeight="1">
-      <c r="A57" s="6"/>
+      <c r="A57" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B57" s="5">
         <v>6.4</v>
       </c>
@@ -5807,7 +5907,9 @@
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="1:7" ht="14" customHeight="1">
-      <c r="A58" s="6"/>
+      <c r="A58" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B58" s="5">
         <v>6.5</v>
       </c>
@@ -5822,7 +5924,9 @@
       <c r="G58" s="4"/>
     </row>
     <row r="59" spans="1:7" ht="14" customHeight="1">
-      <c r="A59" s="6"/>
+      <c r="A59" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B59" s="5">
         <v>6.6</v>
       </c>
@@ -5837,7 +5941,9 @@
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="1:7" ht="14" customHeight="1">
-      <c r="A60" s="6"/>
+      <c r="A60" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B60" s="5">
         <v>6.7</v>
       </c>
@@ -5852,7 +5958,9 @@
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="1:7" ht="14" customHeight="1">
-      <c r="A61" s="6"/>
+      <c r="A61" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B61" s="5">
         <v>6.8</v>
       </c>
@@ -5867,7 +5975,9 @@
       <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" ht="14" customHeight="1">
-      <c r="A62" s="6"/>
+      <c r="A62" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B62" s="5">
         <v>6.9</v>
       </c>
@@ -5882,7 +5992,9 @@
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7" ht="14" customHeight="1">
-      <c r="A63" s="6"/>
+      <c r="A63" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B63" s="7">
         <v>6.1</v>
       </c>
@@ -5897,7 +6009,9 @@
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" ht="14" customHeight="1">
-      <c r="A64" s="6"/>
+      <c r="A64" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B64" s="6"/>
       <c r="C64" s="4" t="s">
         <v>186</v>
@@ -5910,7 +6024,9 @@
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" ht="14" customHeight="1">
-      <c r="A65" s="6"/>
+      <c r="A65" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B65" s="6"/>
       <c r="C65" s="4" t="s">
         <v>187</v>
@@ -5923,7 +6039,9 @@
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7" ht="14" customHeight="1">
-      <c r="A66" s="6"/>
+      <c r="A66" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B66" s="6"/>
       <c r="C66" s="4" t="s">
         <v>188</v>
@@ -5936,7 +6054,9 @@
       <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" ht="14" customHeight="1">
-      <c r="A67" s="6"/>
+      <c r="A67" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B67" s="5">
         <v>6.11</v>
       </c>
@@ -5951,7 +6071,9 @@
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" ht="14" customHeight="1">
-      <c r="A68" s="6"/>
+      <c r="A68" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="B68" s="5">
         <v>6.12</v>
       </c>
@@ -5983,7 +6105,9 @@
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="1:7" ht="14" customHeight="1">
-      <c r="A70" s="6"/>
+      <c r="A70" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B70" s="5">
         <v>7.2</v>
       </c>
@@ -5998,7 +6122,9 @@
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7" ht="14" customHeight="1">
-      <c r="A71" s="6"/>
+      <c r="A71" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B71" s="5">
         <v>7.3</v>
       </c>
@@ -6013,7 +6139,9 @@
       <c r="G71" s="4"/>
     </row>
     <row r="72" spans="1:7" ht="14" customHeight="1">
-      <c r="A72" s="6"/>
+      <c r="A72" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B72" s="5">
         <v>7.4</v>
       </c>
@@ -6028,7 +6156,9 @@
       <c r="G72" s="4"/>
     </row>
     <row r="73" spans="1:7" ht="14" customHeight="1">
-      <c r="A73" s="6"/>
+      <c r="A73" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B73" s="6"/>
       <c r="C73" s="4" t="s">
         <v>83</v>
@@ -6041,7 +6171,9 @@
       <c r="G73" s="4"/>
     </row>
     <row r="74" spans="1:7" ht="14" customHeight="1">
-      <c r="A74" s="6"/>
+      <c r="A74" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B74" s="5">
         <v>7.5</v>
       </c>
@@ -6056,7 +6188,9 @@
       <c r="G74" s="4"/>
     </row>
     <row r="75" spans="1:7" ht="14" customHeight="1">
-      <c r="A75" s="6"/>
+      <c r="A75" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B75" s="6"/>
       <c r="C75" s="4" t="s">
         <v>85</v>
@@ -6069,7 +6203,9 @@
       <c r="G75" s="4"/>
     </row>
     <row r="76" spans="1:7" ht="14" customHeight="1">
-      <c r="A76" s="6"/>
+      <c r="A76" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B76" s="6"/>
       <c r="C76" s="4" t="s">
         <v>86</v>
@@ -6082,7 +6218,9 @@
       <c r="G76" s="4"/>
     </row>
     <row r="77" spans="1:7" ht="14" customHeight="1">
-      <c r="A77" s="6"/>
+      <c r="A77" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B77" s="6"/>
       <c r="C77" s="4" t="s">
         <v>87</v>
@@ -6095,7 +6233,9 @@
       <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7" ht="14" customHeight="1">
-      <c r="A78" s="6"/>
+      <c r="A78" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B78" s="6"/>
       <c r="C78" s="4" t="s">
         <v>88</v>
@@ -6108,7 +6248,9 @@
       <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7" ht="14" customHeight="1">
-      <c r="A79" s="6"/>
+      <c r="A79" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B79" s="5">
         <v>7.6</v>
       </c>
@@ -6123,7 +6265,9 @@
       <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" ht="14" customHeight="1">
-      <c r="A80" s="6"/>
+      <c r="A80" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B80" s="6"/>
       <c r="C80" s="4" t="s">
         <v>90</v>
@@ -6136,7 +6280,9 @@
       <c r="G80" s="4"/>
     </row>
     <row r="81" spans="1:7" ht="14" customHeight="1">
-      <c r="A81" s="6"/>
+      <c r="A81" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B81" s="6"/>
       <c r="C81" s="4" t="s">
         <v>91</v>
@@ -6149,7 +6295,9 @@
       <c r="G81" s="4"/>
     </row>
     <row r="82" spans="1:7" ht="14" customHeight="1">
-      <c r="A82" s="6"/>
+      <c r="A82" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B82" s="6"/>
       <c r="C82" s="4" t="s">
         <v>92</v>
@@ -6162,7 +6310,9 @@
       <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7" ht="14" customHeight="1">
-      <c r="A83" s="6"/>
+      <c r="A83" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B83" s="6"/>
       <c r="C83" s="4" t="s">
         <v>93</v>
@@ -6175,7 +6325,9 @@
       <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7" ht="14" customHeight="1">
-      <c r="A84" s="6"/>
+      <c r="A84" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="B84" s="5">
         <v>7.7</v>
       </c>
@@ -6207,7 +6359,9 @@
       <c r="G85" s="4"/>
     </row>
     <row r="86" spans="1:7" ht="14" customHeight="1">
-      <c r="A86" s="6"/>
+      <c r="A86" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B86" s="6"/>
       <c r="C86" s="4" t="s">
         <v>195</v>
@@ -6220,7 +6374,9 @@
       <c r="G86" s="4"/>
     </row>
     <row r="87" spans="1:7" ht="14" customHeight="1">
-      <c r="A87" s="6"/>
+      <c r="A87" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B87" s="6"/>
       <c r="C87" s="4" t="s">
         <v>196</v>
@@ -6233,7 +6389,9 @@
       <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7" ht="14" customHeight="1">
-      <c r="A88" s="6"/>
+      <c r="A88" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B88" s="5">
         <v>8.1999999999999993</v>
       </c>
@@ -6248,7 +6406,9 @@
       <c r="G88" s="4"/>
     </row>
     <row r="89" spans="1:7" ht="14" customHeight="1">
-      <c r="A89" s="6"/>
+      <c r="A89" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B89" s="6"/>
       <c r="C89" s="4" t="s">
         <v>198</v>
@@ -6261,7 +6421,9 @@
       <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7" ht="14" customHeight="1">
-      <c r="A90" s="6"/>
+      <c r="A90" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B90" s="5">
         <v>8.3000000000000007</v>
       </c>
@@ -6276,7 +6438,9 @@
       <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" ht="14" customHeight="1">
-      <c r="A91" s="6"/>
+      <c r="A91" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B91" s="6"/>
       <c r="C91" s="4" t="s">
         <v>200</v>
@@ -6289,7 +6453,9 @@
       <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7" ht="14" customHeight="1">
-      <c r="A92" s="6"/>
+      <c r="A92" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B92" s="6"/>
       <c r="C92" s="4" t="s">
         <v>201</v>
@@ -6302,7 +6468,9 @@
       <c r="G92" s="4"/>
     </row>
     <row r="93" spans="1:7" ht="14" customHeight="1">
-      <c r="A93" s="6"/>
+      <c r="A93" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B93" s="5">
         <v>8.4</v>
       </c>
@@ -6317,7 +6485,9 @@
       <c r="G93" s="4"/>
     </row>
     <row r="94" spans="1:7" ht="14" customHeight="1">
-      <c r="A94" s="6"/>
+      <c r="A94" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="B94" s="6"/>
       <c r="C94" s="4" t="s">
         <v>203</v>
@@ -6347,7 +6517,9 @@
       <c r="G95" s="4"/>
     </row>
     <row r="96" spans="1:7" ht="14" customHeight="1">
-      <c r="A96" s="6"/>
+      <c r="A96" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B96" s="6"/>
       <c r="C96" s="4" t="s">
         <v>205</v>
@@ -6360,7 +6532,9 @@
       <c r="G96" s="4"/>
     </row>
     <row r="97" spans="1:7" ht="14" customHeight="1">
-      <c r="A97" s="6"/>
+      <c r="A97" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B97" s="5">
         <v>9.1999999999999993</v>
       </c>
@@ -6375,7 +6549,9 @@
       <c r="G97" s="4"/>
     </row>
     <row r="98" spans="1:7" ht="14" customHeight="1">
-      <c r="A98" s="6"/>
+      <c r="A98" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B98" s="6"/>
       <c r="C98" s="4" t="s">
         <v>207</v>
@@ -6388,7 +6564,9 @@
       <c r="G98" s="4"/>
     </row>
     <row r="99" spans="1:7" ht="14" customHeight="1">
-      <c r="A99" s="6"/>
+      <c r="A99" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B99" s="5">
         <v>9.3000000000000007</v>
       </c>
@@ -6403,7 +6581,9 @@
       <c r="G99" s="4"/>
     </row>
     <row r="100" spans="1:7" ht="14" customHeight="1">
-      <c r="A100" s="6"/>
+      <c r="A100" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="B100" s="5">
         <v>9.4</v>
       </c>
@@ -6435,7 +6615,9 @@
       <c r="G101" s="4"/>
     </row>
     <row r="102" spans="1:7" ht="14" customHeight="1">
-      <c r="A102" s="6"/>
+      <c r="A102" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B102" s="6"/>
       <c r="C102" s="4" t="s">
         <v>211</v>
@@ -6448,7 +6630,9 @@
       <c r="G102" s="4"/>
     </row>
     <row r="103" spans="1:7" ht="14" customHeight="1">
-      <c r="A103" s="6"/>
+      <c r="A103" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B103" s="5">
         <v>10.199999999999999</v>
       </c>
@@ -6463,7 +6647,9 @@
       <c r="G103" s="4"/>
     </row>
     <row r="104" spans="1:7" ht="14" customHeight="1">
-      <c r="A104" s="6"/>
+      <c r="A104" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B104" s="6"/>
       <c r="C104" s="4" t="s">
         <v>213</v>
@@ -6476,7 +6662,9 @@
       <c r="G104" s="4"/>
     </row>
     <row r="105" spans="1:7" ht="14" customHeight="1">
-      <c r="A105" s="6"/>
+      <c r="A105" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B105" s="5">
         <v>10.3</v>
       </c>
@@ -6491,7 +6679,9 @@
       <c r="G105" s="4"/>
     </row>
     <row r="106" spans="1:7" ht="14" customHeight="1">
-      <c r="A106" s="6"/>
+      <c r="A106" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B106" s="6"/>
       <c r="C106" s="4" t="s">
         <v>215</v>
@@ -6504,7 +6694,9 @@
       <c r="G106" s="4"/>
     </row>
     <row r="107" spans="1:7" ht="14" customHeight="1">
-      <c r="A107" s="6"/>
+      <c r="A107" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B107" s="5">
         <v>10.4</v>
       </c>
@@ -6519,7 +6711,9 @@
       <c r="G107" s="4"/>
     </row>
     <row r="108" spans="1:7" ht="14" customHeight="1">
-      <c r="A108" s="6"/>
+      <c r="A108" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B108" s="6"/>
       <c r="C108" s="4" t="s">
         <v>217</v>
@@ -6532,7 +6726,9 @@
       <c r="G108" s="4"/>
     </row>
     <row r="109" spans="1:7" ht="14" customHeight="1">
-      <c r="A109" s="6"/>
+      <c r="A109" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B109" s="5">
         <v>10.5</v>
       </c>
@@ -6547,7 +6743,9 @@
       <c r="G109" s="4"/>
     </row>
     <row r="110" spans="1:7" ht="14" customHeight="1">
-      <c r="A110" s="6"/>
+      <c r="A110" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B110" s="6"/>
       <c r="C110" s="4" t="s">
         <v>219</v>
@@ -6560,7 +6758,9 @@
       <c r="G110" s="4"/>
     </row>
     <row r="111" spans="1:7" ht="14" customHeight="1">
-      <c r="A111" s="6"/>
+      <c r="A111" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B111" s="6"/>
       <c r="C111" s="4" t="s">
         <v>220</v>
@@ -6573,7 +6773,9 @@
       <c r="G111" s="4"/>
     </row>
     <row r="112" spans="1:7" ht="14" customHeight="1">
-      <c r="A112" s="6"/>
+      <c r="A112" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B112" s="6"/>
       <c r="C112" s="4" t="s">
         <v>221</v>
@@ -6586,7 +6788,9 @@
       <c r="G112" s="4"/>
     </row>
     <row r="113" spans="1:7" ht="14" customHeight="1">
-      <c r="A113" s="6"/>
+      <c r="A113" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B113" s="5">
         <v>10.6</v>
       </c>
@@ -6601,7 +6805,9 @@
       <c r="G113" s="4"/>
     </row>
     <row r="114" spans="1:7" ht="14" customHeight="1">
-      <c r="A114" s="6"/>
+      <c r="A114" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B114" s="6"/>
       <c r="C114" s="4" t="s">
         <v>223</v>
@@ -6614,7 +6820,9 @@
       <c r="G114" s="4"/>
     </row>
     <row r="115" spans="1:7" ht="14" customHeight="1">
-      <c r="A115" s="6"/>
+      <c r="A115" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B115" s="6"/>
       <c r="C115" s="4" t="s">
         <v>224</v>
@@ -6627,7 +6835,9 @@
       <c r="G115" s="4"/>
     </row>
     <row r="116" spans="1:7" ht="14" customHeight="1">
-      <c r="A116" s="6"/>
+      <c r="A116" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B116" s="6"/>
       <c r="C116" s="4" t="s">
         <v>225</v>
@@ -6640,7 +6850,9 @@
       <c r="G116" s="4"/>
     </row>
     <row r="117" spans="1:7" ht="14" customHeight="1">
-      <c r="A117" s="6"/>
+      <c r="A117" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B117" s="6"/>
       <c r="C117" s="4" t="s">
         <v>226</v>
@@ -6653,7 +6865,9 @@
       <c r="G117" s="4"/>
     </row>
     <row r="118" spans="1:7" ht="14" customHeight="1">
-      <c r="A118" s="6"/>
+      <c r="A118" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B118" s="6"/>
       <c r="C118" s="4" t="s">
         <v>227</v>
@@ -6666,7 +6880,9 @@
       <c r="G118" s="4"/>
     </row>
     <row r="119" spans="1:7" ht="14" customHeight="1">
-      <c r="A119" s="6"/>
+      <c r="A119" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B119" s="5">
         <v>10.7</v>
       </c>
@@ -6681,7 +6897,9 @@
       <c r="G119" s="4"/>
     </row>
     <row r="120" spans="1:7" ht="14" customHeight="1">
-      <c r="A120" s="6"/>
+      <c r="A120" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B120" s="6"/>
       <c r="C120" s="4" t="s">
         <v>229</v>
@@ -6694,7 +6912,9 @@
       <c r="G120" s="4"/>
     </row>
     <row r="121" spans="1:7" ht="14" customHeight="1">
-      <c r="A121" s="6"/>
+      <c r="A121" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="B121" s="5">
         <v>10.8</v>
       </c>
@@ -6726,7 +6946,9 @@
       <c r="G122" s="4"/>
     </row>
     <row r="123" spans="1:7" ht="14" customHeight="1">
-      <c r="A123" s="6"/>
+      <c r="A123" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="B123" s="5">
         <v>11.2</v>
       </c>
@@ -6741,7 +6963,9 @@
       <c r="G123" s="4"/>
     </row>
     <row r="124" spans="1:7" ht="14" customHeight="1">
-      <c r="A124" s="6"/>
+      <c r="A124" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="B124" s="5">
         <v>11.3</v>
       </c>

</xml_diff>

<commit_message>
OA system update and big changes
</commit_message>
<xml_diff>
--- a/final/data/VendorPriceSheet.xlsx
+++ b/final/data/VendorPriceSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangjiaqian/Desktop/git/1/final/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0335D324-AC39-084E-80A6-40C7974648B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AE68D4-88CA-1B45-9431-B852E04AD2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14320" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="600" windowWidth="14320" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="中文" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="293">
   <si>
     <t>Category</t>
   </si>
@@ -1091,6 +1091,10 @@
   </si>
   <si>
     <t>Quantity</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flooring</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4955,7 +4959,7 @@
   <dimension ref="A1:IV126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" customHeight="1"/>
@@ -4991,8 +4995,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="14" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
+      <c r="A2" s="10" t="s">
+        <v>292</v>
       </c>
       <c r="B2" s="5">
         <v>1.1000000000000001</v>

</xml_diff>